<commit_message>
Inserted  data to database
</commit_message>
<xml_diff>
--- a/Module1/task1/DataForImportPro.xlsx
+++ b/Module1/task1/DataForImportPro.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16485" windowHeight="8985" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16485" windowHeight="8985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Truck" sheetId="1" r:id="rId1"/>
     <sheet name="Driver" sheetId="2" r:id="rId2"/>
-    <sheet name="TruckAndDriver" sheetId="5" r:id="rId3"/>
-    <sheet name="Warehouse" sheetId="3" r:id="rId4"/>
-    <sheet name="Cargo" sheetId="6" r:id="rId5"/>
-    <sheet name="Routes" sheetId="4" r:id="rId6"/>
+    <sheet name="Customer" sheetId="7" r:id="rId3"/>
+    <sheet name="TruckAndDriver" sheetId="5" r:id="rId4"/>
+    <sheet name="Warehouse" sheetId="3" r:id="rId5"/>
+    <sheet name="Cargo" sheetId="6" r:id="rId6"/>
+    <sheet name="Route" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Warehouse!$A$1:$C$296</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Warehouse!$A$1:$C$296</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="410">
   <si>
     <t>Brand</t>
   </si>
@@ -1259,6 +1260,9 @@
   </si>
   <si>
     <t>DestinationWharehouseId</t>
+  </si>
+  <si>
+    <t>CustomerId</t>
   </si>
 </sst>
 </file>
@@ -1985,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,9 +2327,321 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="B1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="2">
+        <v>28235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2">
+        <v>29678</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="2">
+        <v>27412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="2">
+        <v>23561</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="2">
+        <v>31771</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="2">
+        <v>13260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2">
+        <v>30067</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="2">
+        <v>20182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2">
+        <v>19100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="2">
+        <v>31074</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="2">
+        <v>28479</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2">
+        <v>27559</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2">
+        <v>30067</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2">
+        <v>27495</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="2">
+        <v>31327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2">
+        <v>31771</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="2">
+        <v>24495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2">
+        <v>27537</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="2">
+        <v>29295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2">
+        <v>31138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -2531,11 +2847,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C296"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -6366,7 +6682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -6605,12 +6921,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C591"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6640,7 +6956,7 @@
       </c>
       <c r="C2">
         <f ca="1">CEILING(RAND()* 1000, 1)</f>
-        <v>58</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6652,7 +6968,7 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C11" ca="1" si="0">CEILING(RAND()* 1000, 1)</f>
-        <v>378</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -6664,7 +6980,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>910</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -6676,7 +6992,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>642</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6688,7 +7004,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>762</v>
+        <v>714</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6700,7 +7016,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>867</v>
+        <v>503</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6712,7 +7028,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>704</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6724,7 +7040,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6736,7 +7052,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>313</v>
+        <v>728</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6748,7 +7064,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>747</v>
+        <v>606</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -6760,7 +7076,7 @@
       </c>
       <c r="C12">
         <f t="shared" ref="C12:C66" ca="1" si="1">CEILING(RAND()* 1000, 1)</f>
-        <v>913</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -6772,7 +7088,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>238</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -6784,7 +7100,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>757</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -6796,7 +7112,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>894</v>
+        <v>852</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -6808,7 +7124,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>936</v>
+        <v>836</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -6820,7 +7136,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>195</v>
+        <v>477</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6832,7 +7148,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>909</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6844,7 +7160,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>587</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6856,7 +7172,7 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>786</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -6868,7 +7184,7 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>995</v>
+        <v>501</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6880,7 +7196,7 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>875</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -6892,7 +7208,7 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>854</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6904,7 +7220,7 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>221</v>
+        <v>481</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -6916,7 +7232,7 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>691</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -6928,7 +7244,7 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>836</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -6940,7 +7256,7 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>145</v>
+        <v>745</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -6952,7 +7268,7 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>587</v>
+        <v>470</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -6964,7 +7280,7 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>965</v>
+        <v>436</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -6976,7 +7292,7 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>595</v>
+        <v>619</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -6988,7 +7304,7 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="1"/>
-        <v>364</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -7000,7 +7316,7 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>528</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -7012,7 +7328,7 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="1"/>
-        <v>990</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -7024,7 +7340,7 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="1"/>
-        <v>367</v>
+        <v>778</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -7036,7 +7352,7 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="1"/>
-        <v>274</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -7048,7 +7364,7 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>977</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -7060,7 +7376,7 @@
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="1"/>
-        <v>714</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -7072,7 +7388,7 @@
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="1"/>
-        <v>601</v>
+        <v>428</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -7084,7 +7400,7 @@
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="1"/>
-        <v>838</v>
+        <v>740</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -7096,7 +7412,7 @@
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="1"/>
-        <v>180</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -7108,7 +7424,7 @@
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="1"/>
-        <v>541</v>
+        <v>468</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -7120,7 +7436,7 @@
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="1"/>
-        <v>904</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -7132,7 +7448,7 @@
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="1"/>
-        <v>851</v>
+        <v>612</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -7144,7 +7460,7 @@
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="1"/>
-        <v>554</v>
+        <v>745</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -7156,7 +7472,7 @@
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="1"/>
-        <v>545</v>
+        <v>905</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -7168,7 +7484,7 @@
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="1"/>
-        <v>943</v>
+        <v>538</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -7180,7 +7496,7 @@
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="1"/>
-        <v>502</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -7192,7 +7508,7 @@
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="1"/>
-        <v>141</v>
+        <v>321</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -7204,7 +7520,7 @@
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="1"/>
-        <v>373</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -7216,7 +7532,7 @@
       </c>
       <c r="C50">
         <f t="shared" ca="1" si="1"/>
-        <v>598</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -7228,7 +7544,7 @@
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="1"/>
-        <v>252</v>
+        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -7240,7 +7556,7 @@
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="1"/>
-        <v>631</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -7252,7 +7568,7 @@
       </c>
       <c r="C53">
         <f t="shared" ca="1" si="1"/>
-        <v>888</v>
+        <v>416</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -7264,7 +7580,7 @@
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="1"/>
-        <v>414</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -7276,7 +7592,7 @@
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="1"/>
-        <v>264</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -7288,7 +7604,7 @@
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="1"/>
-        <v>999</v>
+        <v>416</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -7300,7 +7616,7 @@
       </c>
       <c r="C57">
         <f t="shared" ca="1" si="1"/>
-        <v>368</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -7312,7 +7628,7 @@
       </c>
       <c r="C58">
         <f t="shared" ca="1" si="1"/>
-        <v>398</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -7324,7 +7640,7 @@
       </c>
       <c r="C59">
         <f t="shared" ca="1" si="1"/>
-        <v>828</v>
+        <v>823</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -7336,7 +7652,7 @@
       </c>
       <c r="C60">
         <f t="shared" ca="1" si="1"/>
-        <v>747</v>
+        <v>433</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -7348,7 +7664,7 @@
       </c>
       <c r="C61">
         <f t="shared" ca="1" si="1"/>
-        <v>197</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -7360,7 +7676,7 @@
       </c>
       <c r="C62">
         <f t="shared" ca="1" si="1"/>
-        <v>579</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -7372,7 +7688,7 @@
       </c>
       <c r="C63">
         <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <v>771</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -7384,7 +7700,7 @@
       </c>
       <c r="C64">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>234</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -7396,7 +7712,7 @@
       </c>
       <c r="C65">
         <f t="shared" ca="1" si="1"/>
-        <v>887</v>
+        <v>889</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -7408,7 +7724,7 @@
       </c>
       <c r="C66">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -7420,7 +7736,7 @@
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C130" ca="1" si="2">CEILING(RAND()* 1000, 1)</f>
-        <v>562</v>
+        <v>639</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -7432,7 +7748,7 @@
       </c>
       <c r="C68">
         <f t="shared" ca="1" si="2"/>
-        <v>844</v>
+        <v>250</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -7444,7 +7760,7 @@
       </c>
       <c r="C69">
         <f t="shared" ca="1" si="2"/>
-        <v>837</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -7456,7 +7772,7 @@
       </c>
       <c r="C70">
         <f t="shared" ca="1" si="2"/>
-        <v>961</v>
+        <v>446</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -7468,7 +7784,7 @@
       </c>
       <c r="C71">
         <f t="shared" ca="1" si="2"/>
-        <v>930</v>
+        <v>882</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -7480,7 +7796,7 @@
       </c>
       <c r="C72">
         <f t="shared" ca="1" si="2"/>
-        <v>200</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -7492,7 +7808,7 @@
       </c>
       <c r="C73">
         <f t="shared" ca="1" si="2"/>
-        <v>734</v>
+        <v>315</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -7504,7 +7820,7 @@
       </c>
       <c r="C74">
         <f t="shared" ca="1" si="2"/>
-        <v>798</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -7516,7 +7832,7 @@
       </c>
       <c r="C75">
         <f t="shared" ca="1" si="2"/>
-        <v>602</v>
+        <v>469</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -7528,7 +7844,7 @@
       </c>
       <c r="C76">
         <f t="shared" ca="1" si="2"/>
-        <v>175</v>
+        <v>961</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -7540,7 +7856,7 @@
       </c>
       <c r="C77">
         <f t="shared" ca="1" si="2"/>
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -7552,7 +7868,7 @@
       </c>
       <c r="C78">
         <f t="shared" ca="1" si="2"/>
-        <v>719</v>
+        <v>614</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -7564,7 +7880,7 @@
       </c>
       <c r="C79">
         <f t="shared" ca="1" si="2"/>
-        <v>501</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -7576,7 +7892,7 @@
       </c>
       <c r="C80">
         <f t="shared" ca="1" si="2"/>
-        <v>984</v>
+        <v>826</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -7588,7 +7904,7 @@
       </c>
       <c r="C81">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>761</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -7600,7 +7916,7 @@
       </c>
       <c r="C82">
         <f t="shared" ca="1" si="2"/>
-        <v>523</v>
+        <v>246</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -7612,7 +7928,7 @@
       </c>
       <c r="C83">
         <f t="shared" ca="1" si="2"/>
-        <v>724</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -7624,7 +7940,7 @@
       </c>
       <c r="C84">
         <f t="shared" ca="1" si="2"/>
-        <v>443</v>
+        <v>400</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -7636,7 +7952,7 @@
       </c>
       <c r="C85">
         <f t="shared" ca="1" si="2"/>
-        <v>366</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -7648,7 +7964,7 @@
       </c>
       <c r="C86">
         <f t="shared" ca="1" si="2"/>
-        <v>306</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -7660,7 +7976,7 @@
       </c>
       <c r="C87">
         <f t="shared" ca="1" si="2"/>
-        <v>841</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -7672,7 +7988,7 @@
       </c>
       <c r="C88">
         <f t="shared" ca="1" si="2"/>
-        <v>363</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -7684,7 +8000,7 @@
       </c>
       <c r="C89">
         <f t="shared" ca="1" si="2"/>
-        <v>701</v>
+        <v>542</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -7696,7 +8012,7 @@
       </c>
       <c r="C90">
         <f t="shared" ca="1" si="2"/>
-        <v>617</v>
+        <v>674</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -7708,7 +8024,7 @@
       </c>
       <c r="C91">
         <f t="shared" ca="1" si="2"/>
-        <v>93</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -7720,7 +8036,7 @@
       </c>
       <c r="C92">
         <f t="shared" ca="1" si="2"/>
-        <v>512</v>
+        <v>616</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -7732,7 +8048,7 @@
       </c>
       <c r="C93">
         <f t="shared" ca="1" si="2"/>
-        <v>610</v>
+        <v>491</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -7744,7 +8060,7 @@
       </c>
       <c r="C94">
         <f t="shared" ca="1" si="2"/>
-        <v>871</v>
+        <v>762</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -7756,7 +8072,7 @@
       </c>
       <c r="C95">
         <f t="shared" ca="1" si="2"/>
-        <v>306</v>
+        <v>485</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -7768,7 +8084,7 @@
       </c>
       <c r="C96">
         <f t="shared" ca="1" si="2"/>
-        <v>951</v>
+        <v>577</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -7780,7 +8096,7 @@
       </c>
       <c r="C97">
         <f t="shared" ca="1" si="2"/>
-        <v>165</v>
+        <v>378</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -7792,7 +8108,7 @@
       </c>
       <c r="C98">
         <f t="shared" ca="1" si="2"/>
-        <v>648</v>
+        <v>582</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -7804,7 +8120,7 @@
       </c>
       <c r="C99">
         <f t="shared" ca="1" si="2"/>
-        <v>584</v>
+        <v>804</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -7816,7 +8132,7 @@
       </c>
       <c r="C100">
         <f t="shared" ca="1" si="2"/>
-        <v>488</v>
+        <v>839</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -7828,7 +8144,7 @@
       </c>
       <c r="C101">
         <f t="shared" ca="1" si="2"/>
-        <v>950</v>
+        <v>916</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -7840,7 +8156,7 @@
       </c>
       <c r="C102">
         <f t="shared" ca="1" si="2"/>
-        <v>140</v>
+        <v>227</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -7852,7 +8168,7 @@
       </c>
       <c r="C103">
         <f t="shared" ca="1" si="2"/>
-        <v>593</v>
+        <v>62</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -7864,7 +8180,7 @@
       </c>
       <c r="C104">
         <f t="shared" ca="1" si="2"/>
-        <v>444</v>
+        <v>233</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -7876,7 +8192,7 @@
       </c>
       <c r="C105">
         <f t="shared" ca="1" si="2"/>
-        <v>298</v>
+        <v>845</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -7888,7 +8204,7 @@
       </c>
       <c r="C106">
         <f t="shared" ca="1" si="2"/>
-        <v>249</v>
+        <v>479</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -7900,7 +8216,7 @@
       </c>
       <c r="C107">
         <f t="shared" ca="1" si="2"/>
-        <v>224</v>
+        <v>314</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -7912,7 +8228,7 @@
       </c>
       <c r="C108">
         <f t="shared" ca="1" si="2"/>
-        <v>588</v>
+        <v>61</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -7924,7 +8240,7 @@
       </c>
       <c r="C109">
         <f t="shared" ca="1" si="2"/>
-        <v>817</v>
+        <v>700</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -7936,7 +8252,7 @@
       </c>
       <c r="C110">
         <f t="shared" ca="1" si="2"/>
-        <v>278</v>
+        <v>296</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -7948,7 +8264,7 @@
       </c>
       <c r="C111">
         <f t="shared" ca="1" si="2"/>
-        <v>160</v>
+        <v>594</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -7960,7 +8276,7 @@
       </c>
       <c r="C112">
         <f t="shared" ca="1" si="2"/>
-        <v>915</v>
+        <v>121</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -7972,7 +8288,7 @@
       </c>
       <c r="C113">
         <f t="shared" ca="1" si="2"/>
-        <v>755</v>
+        <v>256</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -7984,7 +8300,7 @@
       </c>
       <c r="C114">
         <f t="shared" ca="1" si="2"/>
-        <v>86</v>
+        <v>140</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -7996,7 +8312,7 @@
       </c>
       <c r="C115">
         <f t="shared" ca="1" si="2"/>
-        <v>660</v>
+        <v>540</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -8008,7 +8324,7 @@
       </c>
       <c r="C116">
         <f t="shared" ca="1" si="2"/>
-        <v>857</v>
+        <v>253</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -8020,7 +8336,7 @@
       </c>
       <c r="C117">
         <f t="shared" ca="1" si="2"/>
-        <v>340</v>
+        <v>18</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -8032,7 +8348,7 @@
       </c>
       <c r="C118">
         <f t="shared" ca="1" si="2"/>
-        <v>679</v>
+        <v>300</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -8044,7 +8360,7 @@
       </c>
       <c r="C119">
         <f t="shared" ca="1" si="2"/>
-        <v>318</v>
+        <v>769</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -8056,7 +8372,7 @@
       </c>
       <c r="C120">
         <f t="shared" ca="1" si="2"/>
-        <v>634</v>
+        <v>676</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -8068,7 +8384,7 @@
       </c>
       <c r="C121">
         <f t="shared" ca="1" si="2"/>
-        <v>735</v>
+        <v>615</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -8080,7 +8396,7 @@
       </c>
       <c r="C122">
         <f t="shared" ca="1" si="2"/>
-        <v>590</v>
+        <v>286</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -8092,7 +8408,7 @@
       </c>
       <c r="C123">
         <f t="shared" ca="1" si="2"/>
-        <v>697</v>
+        <v>317</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -8104,7 +8420,7 @@
       </c>
       <c r="C124">
         <f t="shared" ca="1" si="2"/>
-        <v>539</v>
+        <v>624</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -8116,7 +8432,7 @@
       </c>
       <c r="C125">
         <f t="shared" ca="1" si="2"/>
-        <v>383</v>
+        <v>757</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -8128,7 +8444,7 @@
       </c>
       <c r="C126">
         <f t="shared" ca="1" si="2"/>
-        <v>971</v>
+        <v>885</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -8140,7 +8456,7 @@
       </c>
       <c r="C127">
         <f t="shared" ca="1" si="2"/>
-        <v>763</v>
+        <v>616</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -8152,7 +8468,7 @@
       </c>
       <c r="C128">
         <f t="shared" ca="1" si="2"/>
-        <v>610</v>
+        <v>740</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -8164,7 +8480,7 @@
       </c>
       <c r="C129">
         <f t="shared" ca="1" si="2"/>
-        <v>230</v>
+        <v>34</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -8176,7 +8492,7 @@
       </c>
       <c r="C130">
         <f t="shared" ca="1" si="2"/>
-        <v>820</v>
+        <v>990</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -8188,7 +8504,7 @@
       </c>
       <c r="C131">
         <f t="shared" ref="C131:C170" ca="1" si="3">CEILING(RAND()* 1000, 1)</f>
-        <v>87</v>
+        <v>344</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -8200,7 +8516,7 @@
       </c>
       <c r="C132">
         <f t="shared" ca="1" si="3"/>
-        <v>354</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -8212,7 +8528,7 @@
       </c>
       <c r="C133">
         <f t="shared" ca="1" si="3"/>
-        <v>206</v>
+        <v>679</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -8224,7 +8540,7 @@
       </c>
       <c r="C134">
         <f t="shared" ca="1" si="3"/>
-        <v>820</v>
+        <v>55</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -8236,7 +8552,7 @@
       </c>
       <c r="C135">
         <f t="shared" ca="1" si="3"/>
-        <v>533</v>
+        <v>694</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -8248,7 +8564,7 @@
       </c>
       <c r="C136">
         <f t="shared" ca="1" si="3"/>
-        <v>338</v>
+        <v>513</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -8260,7 +8576,7 @@
       </c>
       <c r="C137">
         <f t="shared" ca="1" si="3"/>
-        <v>226</v>
+        <v>377</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -8272,7 +8588,7 @@
       </c>
       <c r="C138">
         <f t="shared" ca="1" si="3"/>
-        <v>249</v>
+        <v>789</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -8284,7 +8600,7 @@
       </c>
       <c r="C139">
         <f t="shared" ca="1" si="3"/>
-        <v>25</v>
+        <v>907</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -8296,7 +8612,7 @@
       </c>
       <c r="C140">
         <f t="shared" ca="1" si="3"/>
-        <v>371</v>
+        <v>503</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -8308,7 +8624,7 @@
       </c>
       <c r="C141">
         <f t="shared" ca="1" si="3"/>
-        <v>224</v>
+        <v>558</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -8320,7 +8636,7 @@
       </c>
       <c r="C142">
         <f t="shared" ca="1" si="3"/>
-        <v>363</v>
+        <v>377</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -8332,7 +8648,7 @@
       </c>
       <c r="C143">
         <f t="shared" ca="1" si="3"/>
-        <v>119</v>
+        <v>721</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -8344,7 +8660,7 @@
       </c>
       <c r="C144">
         <f t="shared" ca="1" si="3"/>
-        <v>124</v>
+        <v>287</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -8356,7 +8672,7 @@
       </c>
       <c r="C145">
         <f t="shared" ca="1" si="3"/>
-        <v>454</v>
+        <v>512</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -8368,7 +8684,7 @@
       </c>
       <c r="C146">
         <f t="shared" ca="1" si="3"/>
-        <v>988</v>
+        <v>874</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -8380,7 +8696,7 @@
       </c>
       <c r="C147">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>184</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -8392,7 +8708,7 @@
       </c>
       <c r="C148">
         <f t="shared" ca="1" si="3"/>
-        <v>88</v>
+        <v>177</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -8404,7 +8720,7 @@
       </c>
       <c r="C149">
         <f t="shared" ca="1" si="3"/>
-        <v>393</v>
+        <v>457</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -8416,7 +8732,7 @@
       </c>
       <c r="C150">
         <f t="shared" ca="1" si="3"/>
-        <v>494</v>
+        <v>939</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -8428,7 +8744,7 @@
       </c>
       <c r="C151">
         <f t="shared" ca="1" si="3"/>
-        <v>973</v>
+        <v>325</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -8440,7 +8756,7 @@
       </c>
       <c r="C152">
         <f t="shared" ca="1" si="3"/>
-        <v>84</v>
+        <v>610</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -8452,7 +8768,7 @@
       </c>
       <c r="C153">
         <f t="shared" ca="1" si="3"/>
-        <v>866</v>
+        <v>25</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -8464,7 +8780,7 @@
       </c>
       <c r="C154">
         <f t="shared" ca="1" si="3"/>
-        <v>415</v>
+        <v>998</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -8476,7 +8792,7 @@
       </c>
       <c r="C155">
         <f t="shared" ca="1" si="3"/>
-        <v>907</v>
+        <v>593</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -8488,7 +8804,7 @@
       </c>
       <c r="C156">
         <f t="shared" ca="1" si="3"/>
-        <v>692</v>
+        <v>824</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -8500,7 +8816,7 @@
       </c>
       <c r="C157">
         <f t="shared" ca="1" si="3"/>
-        <v>561</v>
+        <v>271</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -8512,7 +8828,7 @@
       </c>
       <c r="C158">
         <f t="shared" ca="1" si="3"/>
-        <v>222</v>
+        <v>435</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -8524,7 +8840,7 @@
       </c>
       <c r="C159">
         <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>152</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -8536,7 +8852,7 @@
       </c>
       <c r="C160">
         <f t="shared" ca="1" si="3"/>
-        <v>539</v>
+        <v>866</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -8548,7 +8864,7 @@
       </c>
       <c r="C161">
         <f t="shared" ca="1" si="3"/>
-        <v>503</v>
+        <v>536</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -8560,7 +8876,7 @@
       </c>
       <c r="C162">
         <f t="shared" ca="1" si="3"/>
-        <v>706</v>
+        <v>370</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -8572,7 +8888,7 @@
       </c>
       <c r="C163">
         <f t="shared" ca="1" si="3"/>
-        <v>835</v>
+        <v>549</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -8584,7 +8900,7 @@
       </c>
       <c r="C164">
         <f t="shared" ca="1" si="3"/>
-        <v>526</v>
+        <v>541</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -8596,7 +8912,7 @@
       </c>
       <c r="C165">
         <f t="shared" ca="1" si="3"/>
-        <v>779</v>
+        <v>869</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -8608,7 +8924,7 @@
       </c>
       <c r="C166">
         <f t="shared" ca="1" si="3"/>
-        <v>863</v>
+        <v>311</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -8620,7 +8936,7 @@
       </c>
       <c r="C167">
         <f t="shared" ca="1" si="3"/>
-        <v>923</v>
+        <v>287</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -8632,7 +8948,7 @@
       </c>
       <c r="C168">
         <f t="shared" ca="1" si="3"/>
-        <v>741</v>
+        <v>209</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -8644,7 +8960,7 @@
       </c>
       <c r="C169">
         <f t="shared" ca="1" si="3"/>
-        <v>510</v>
+        <v>136</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -8656,7 +8972,7 @@
       </c>
       <c r="C170">
         <f t="shared" ca="1" si="3"/>
-        <v>150</v>
+        <v>493</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>